<commit_message>
swaglabs,valid,invalid credentials,about,add to cart with excel
</commit_message>
<xml_diff>
--- a/test_data/data.xlsx
+++ b/test_data/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>${username}</t>
   </si>
@@ -71,41 +71,50 @@
     <t>${phone_number}</t>
   </si>
   <si>
-    <t>${interest}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard_user </t>
+    <t>l&amp;t</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp@gmail.com </t>
+  </si>
+  <si>
+    <t>patil</t>
+  </si>
+  <si>
+    <t>swati</t>
+  </si>
+  <si>
+    <t>2-10</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>${p}</t>
   </si>
   <si>
     <t>secret_sauce</t>
   </si>
   <si>
-    <t xml:space="preserve"> sam</t>
-  </si>
-  <si>
-    <t>anu</t>
-  </si>
-  <si>
-    <t>l&amp;t</t>
-  </si>
-  <si>
-    <t>sm@gmail.com</t>
-  </si>
-  <si>
-    <t>Just Me</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Mobile Testing</t>
+    <t>9987656789</t>
+  </si>
+  <si>
+    <t>uk@gmail.com</t>
+  </si>
+  <si>
+    <t>koti</t>
+  </si>
+  <si>
+    <t>usha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -123,6 +132,13 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,7 +165,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -158,6 +174,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -371,7 +388,9 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -433,95 +452,118 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="3"/>
-    <col min="9" max="9" width="17" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="17" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F1" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25.5">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="3">
+        <v>3454565758</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="I2" s="3">
-        <v>3454565758</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>